<commit_message>
Fixed laptop click interaction & player crouch & added assets credit
</commit_message>
<xml_diff>
--- a/Assets/Design Documents/Assets.xlsx
+++ b/Assets/Design Documents/Assets.xlsx
@@ -1,42 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_7D4755BF84DCCED3EB544A1A8531F45B8AF31AA5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB47BF91-814D-4BF0-81EE-6EB7D2EBAC6B}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letis\Projects\UnityProjects\interactive-classroom-experience\Assets\Design Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196449A8-A02F-4826-8E4F-7BE503A1104A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4428" yWindow="1176" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credits" sheetId="1" r:id="rId1"/>
     <sheet name="Assets" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Assets!$A$1:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Assets!$A$1:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Credits!$A$1:$F$19</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
   <si>
     <t>Use</t>
   </si>
@@ -236,36 +230,15 @@
     <t>Custom emissive material for chandelier lamp</t>
   </si>
   <si>
-    <t>LightSwitch Script</t>
-  </si>
-  <si>
     <t>C# Script</t>
   </si>
   <si>
     <t>.css</t>
   </si>
   <si>
-    <t>Toggles ceiling light ON/OFF when pressing E</t>
-  </si>
-  <si>
-    <t>Not ready yet</t>
-  </si>
-  <si>
     <t>Audio</t>
   </si>
   <si>
-    <t>Classroom Music Trigger Script</t>
-  </si>
-  <si>
-    <t>Plays or stops background music when near headphones</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>Notebook Script</t>
-  </si>
-  <si>
     <t>Opens notebook UI panel to show text</t>
   </si>
   <si>
@@ -279,13 +252,82 @@
   </si>
   <si>
     <t>Interactive Classroom Experience main environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skyboxes </t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/2d/textures-materials/sky/10-skyboxes-pack-day-night-32236?srsltid=AfmBOooh5s-LtcINhJzFBIuWCVWzb3vyiXIEbdEeg26uCsSPz8jT1IUi</t>
+  </si>
+  <si>
+    <t>MP3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nUsHboYC5zc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=koI6xFoRxjg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/AbRGcYP8iBM?si=_WD77-xcBDLvdQ7c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rYoZgpAEkFs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4MgPNabO_g4?si=OLja4Id5OcAMWeEk</t>
+  </si>
+  <si>
+    <t>Free / No Copyright</t>
+  </si>
+  <si>
+    <t>Click Sound</t>
+  </si>
+  <si>
+    <t>Keyboard Typing Sound</t>
+  </si>
+  <si>
+    <t>French Songs</t>
+  </si>
+  <si>
+    <t>Nasheed Jannah Song</t>
+  </si>
+  <si>
+    <t>Birds Sound</t>
+  </si>
+  <si>
+    <t>With the help of AI</t>
+  </si>
+  <si>
+    <t>NotebookInteraction</t>
+  </si>
+  <si>
+    <t>SimplePlayerController</t>
+  </si>
+  <si>
+    <t>TriggerEvent</t>
+  </si>
+  <si>
+    <t>LightSwitchInteraction</t>
+  </si>
+  <si>
+    <t>LaptopClickInteraction</t>
+  </si>
+  <si>
+    <t>DoorAutoOpen</t>
+  </si>
+  <si>
+    <t>DayNightSwitch</t>
+  </si>
+  <si>
+    <t>The final end result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,7 +380,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -670,23 +712,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -726,7 +768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -746,7 +788,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -766,7 +808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -786,7 +828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -806,7 +848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -826,7 +868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -846,7 +888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -866,7 +908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -886,7 +928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -906,7 +948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -926,7 +968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -946,7 +988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -966,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -986,7 +1028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1006,7 +1048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1026,7 +1068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1046,7 +1088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1064,6 +1106,126 @@
       </c>
       <c r="F19" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1094,24 +1256,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="50.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1299,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1160,18 +1322,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
       </c>
       <c r="E3" t="s">
         <v>63</v>
@@ -1183,21 +1342,18 @@
         <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -1205,25 +1361,19 @@
       <c r="F4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
       <c r="H4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
         <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
@@ -1231,25 +1381,19 @@
       <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" t="s">
-        <v>76</v>
-      </c>
       <c r="H5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>63</v>
@@ -1257,15 +1401,98 @@
       <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="G6" t="s">
-        <v>80</v>
-      </c>
       <c r="H6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>70</v>
       </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G6" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}"/>
+  <autoFilter ref="A1:G4" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final excel assets & credits
</commit_message>
<xml_diff>
--- a/Assets/Design Documents/Assets.xlsx
+++ b/Assets/Design Documents/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letis\Projects\UnityProjects\interactive-classroom-experience\Assets\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196449A8-A02F-4826-8E4F-7BE503A1104A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8FBFDA-84E7-4248-BE8B-E20A19EE7B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4428" yWindow="1176" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credits" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="111">
   <si>
     <t>Use</t>
   </si>
@@ -59,9 +59,6 @@
     <t>3D Model</t>
   </si>
   <si>
-    <t>FBX</t>
-  </si>
-  <si>
     <t>https://www.cgtrader.com/free-3d-models/furniture/other/whiteboard-low-poly-pbr</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Texture Pack</t>
   </si>
   <si>
-    <t>PNG</t>
-  </si>
-  <si>
     <t>https://assetstore.unity.com/packages/2d/textures-materials/4k-tiled-ground-textures-part-2-283704</t>
   </si>
   <si>
@@ -233,15 +227,9 @@
     <t>C# Script</t>
   </si>
   <si>
-    <t>.css</t>
-  </si>
-  <si>
     <t>Audio</t>
   </si>
   <si>
-    <t>Opens notebook UI panel to show text</t>
-  </si>
-  <si>
     <t>Scene Setup</t>
   </si>
   <si>
@@ -260,9 +248,6 @@
     <t>https://assetstore.unity.com/packages/2d/textures-materials/sky/10-skyboxes-pack-day-night-32236?srsltid=AfmBOooh5s-LtcINhJzFBIuWCVWzb3vyiXIEbdEeg26uCsSPz8jT1IUi</t>
   </si>
   <si>
-    <t>MP3</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=nUsHboYC5zc</t>
   </si>
   <si>
@@ -321,13 +306,70 @@
   </si>
   <si>
     <t>The final end result</t>
+  </si>
+  <si>
+    <t>.cs</t>
+  </si>
+  <si>
+    <t>Opens and closes the notebook UI panel so the player can read the note</t>
+  </si>
+  <si>
+    <t>First-person controller for walking, jumping and crouching inside the classroom</t>
+  </si>
+  <si>
+    <t>Generic trigger script that invokes UnityEvents when the Player enters or exits a trigger zone</t>
+  </si>
+  <si>
+    <t>Toggles the chandelier lights and plays a click sound when the player presses the interact key near the light switch</t>
+  </si>
+  <si>
+    <t>Lets the player toggle the laptop screen on/off with a left mouse click and plays a typing sound while it is on</t>
+  </si>
+  <si>
+    <t>Switches between day and night skyboxes and enables/disables the Sun light to change the time of day</t>
+  </si>
+  <si>
+    <t>Environment / Lighting</t>
+  </si>
+  <si>
+    <t>Interaction / Events</t>
+  </si>
+  <si>
+    <t>Player / Movement</t>
+  </si>
+  <si>
+    <t>Welcome Audio</t>
+  </si>
+  <si>
+    <t>Audio Clip</t>
+  </si>
+  <si>
+    <t>.mp3</t>
+  </si>
+  <si>
+    <t>Created via Speechma</t>
+  </si>
+  <si>
+    <t>AI-generated voice line welcoming the user to the classroom</t>
+  </si>
+  <si>
+    <t>Custom text-to-speech audio</t>
+  </si>
+  <si>
+    <t>Automatically opens and closes the movable door when the Player enters or leaves the door trigger and can play a welcome audio</t>
+  </si>
+  <si>
+    <t>.png</t>
+  </si>
+  <si>
+    <t>.fbx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +393,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0A0A0A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -373,10 +421,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -715,7 +764,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,14 +807,14 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,99 +822,99 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="D3" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
+      <c r="D4" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="D5" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
+      <c r="D6" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
+      <c r="D7" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -873,239 +922,239 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
+      <c r="D8" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
+      <c r="D9" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
-        <v>9</v>
+      <c r="D10" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>9</v>
+      <c r="D11" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
+      <c r="D12" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
+      <c r="D13" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
-        <v>9</v>
+      <c r="D14" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
+      <c r="D15" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
-        <v>9</v>
+      <c r="D16" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
+      <c r="D18" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
+      <c r="D19" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1113,99 +1162,99 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
         <v>77</v>
-      </c>
-      <c r="F21" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
         <v>76</v>
       </c>
-      <c r="E24" t="s">
-        <v>81</v>
-      </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1213,19 +1262,19 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1251,26 +1300,28 @@
     <hyperlink ref="E19" r:id="rId18" xr:uid="{04097B7D-C4A9-4EA4-ADF5-5453F4656D9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1293,176 +1344,215 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="D9" t="s">
         <v>92</v>
       </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>108</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1470,25 +1560,51 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OutdoorSound & BlackScreen Material Laptop & WelcomeScreen Interaction & Refactored and fixed other interactions
</commit_message>
<xml_diff>
--- a/Assets/Design Documents/Assets.xlsx
+++ b/Assets/Design Documents/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letis\Projects\UnityProjects\interactive-classroom-experience\Assets\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8FBFDA-84E7-4248-BE8B-E20A19EE7B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE01E43D-A8E9-4487-B99B-C4EE77DCF886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credits" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="113">
   <si>
     <t>Use</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>.fbx</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Dk_0rf2YYCw</t>
+  </si>
+  <si>
+    <t>Outdoor Sound</t>
   </si>
 </sst>
 </file>
@@ -761,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,6 +1280,26 @@
         <v>75</v>
       </c>
       <c r="F25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1308,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated Assets (Credits) of Design Documents
</commit_message>
<xml_diff>
--- a/Assets/Design Documents/Assets.xlsx
+++ b/Assets/Design Documents/Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letis\Projects\UnityProjects\interactive-classroom-experience\Assets\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE01E43D-A8E9-4487-B99B-C4EE77DCF886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C352E18-C274-459E-9776-9ACD25DE5366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="114">
   <si>
     <t>Use</t>
   </si>
@@ -254,15 +254,9 @@
     <t>https://www.youtube.com/watch?v=koI6xFoRxjg</t>
   </si>
   <si>
-    <t>https://youtu.be/AbRGcYP8iBM?si=_WD77-xcBDLvdQ7c</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=rYoZgpAEkFs</t>
   </si>
   <si>
-    <t>https://youtu.be/4MgPNabO_g4?si=OLja4Id5OcAMWeEk</t>
-  </si>
-  <si>
     <t>Free / No Copyright</t>
   </si>
   <si>
@@ -369,6 +363,15 @@
   </si>
   <si>
     <t>Outdoor Sound</t>
+  </si>
+  <si>
+    <t>Cutted</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Hi7Rx3En7-k?si=_pQmuayGLrxNr-ES</t>
+  </si>
+  <si>
+    <t>https://youtu.be/UdTzq4pnB6o?si=EutW5CCz8_l58VcB</t>
   </si>
 </sst>
 </file>
@@ -767,7 +770,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
@@ -781,9 +784,10 @@
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="105.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,8 +806,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -814,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -823,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -834,7 +841,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -843,7 +850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -854,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -863,7 +870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -874,7 +881,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
@@ -883,7 +890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -894,7 +901,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -903,7 +910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -914,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>26</v>
@@ -923,7 +930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -934,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
@@ -943,7 +950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -954,7 +961,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -963,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -974,7 +981,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>32</v>
@@ -983,7 +990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -994,7 +1001,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>35</v>
@@ -1003,7 +1010,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1021,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>37</v>
@@ -1023,7 +1030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1041,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>39</v>
@@ -1043,7 +1050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>42</v>
@@ -1063,7 +1070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1074,7 +1081,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>44</v>
@@ -1083,7 +1090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1094,7 +1101,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>47</v>
@@ -1103,7 +1110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>51</v>
@@ -1123,7 +1130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1134,7 +1141,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>53</v>
@@ -1143,7 +1150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>55</v>
@@ -1163,7 +1170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1174,7 +1181,7 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
         <v>71</v>
@@ -1183,124 +1190,127 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
         <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
         <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" t="s">
-        <v>74</v>
+        <v>102</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
         <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
         <v>75</v>
       </c>
-      <c r="F25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
         <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1324,9 +1334,10 @@
     <hyperlink ref="E17" r:id="rId16" xr:uid="{50C3AB93-403E-4E19-8CF9-44795C865209}"/>
     <hyperlink ref="E18" r:id="rId17" xr:uid="{DF2B3BF2-83F6-4F04-A4F4-5528D3C8E59A}"/>
     <hyperlink ref="E19" r:id="rId18" xr:uid="{04097B7D-C4A9-4EA4-ADF5-5453F4656D9E}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{5722DE31-4837-411E-8E19-50F6979AA04C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -1335,7 +1346,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,13 +1415,13 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
@@ -1419,24 +1430,24 @@
         <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
         <v>61</v>
@@ -1445,24 +1456,24 @@
         <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
         <v>61</v>
@@ -1471,10 +1482,10 @@
         <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1482,13 +1493,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>61</v>
@@ -1497,10 +1508,10 @@
         <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1508,13 +1519,13 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
         <v>61</v>
@@ -1523,24 +1534,24 @@
         <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
         <v>61</v>
@@ -1549,10 +1560,10 @@
         <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1560,13 +1571,13 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
         <v>61</v>
@@ -1575,10 +1586,10 @@
         <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1604,7 +1615,7 @@
         <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1612,25 +1623,25 @@
         <v>65</v>
       </c>
       <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
         <v>102</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>103</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" t="s">
-        <v>105</v>
       </c>
       <c r="F11" t="s">
         <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>